<commit_message>
Updated the similarity comparison function
Find the general comparison function at the top of main.py.
</commit_message>
<xml_diff>
--- a/Code/BestModels_DivideBy30.xlsx
+++ b/Code/BestModels_DivideBy30.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -604,295 +604,295 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.9907407407407407</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9539375928677564</v>
+        <v>0.9390787518573551</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4038461538461539</v>
+        <v>0.3970588235294117</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7777777777777778</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.865857685322767</v>
+        <v>0.9695393759286776</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9471428571428572</v>
+        <v>0.9414285714285714</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5316455696202531</v>
+        <v>0.5684210526315789</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>('Divisible_by_8=True', 'Divisible_by_10=True')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_5=True')</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]]</t>
+          <t>df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_8=True AND Divisible_by_10=True</t>
+          <t>Divisible_by_2=True AND Divisible_by_5=True</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.9892141756548536</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9539375928677564</v>
+        <v>0.9390787518573551</v>
       </c>
       <c r="C6" t="n">
-        <v>0.392156862745098</v>
+        <v>0.3970588235294117</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7407407407407407</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8473391668042485</v>
+        <v>0.9695393759286776</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9457142857142857</v>
+        <v>0.9414285714285714</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5128205128205128</v>
+        <v>0.5684210526315789</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>('Divisible_by_7=True', 'Divisible_by_10=True')</t>
+          <t>('Divisible_by_10=True', 'Number∈(2.999, 68.6]')</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_7=True AND Divisible_by_10=True</t>
+          <t>Divisible_by_10=True AND NOT_Number∈(2.999, 68.6 OR Divisible_by_10=True AND Number∈(2.999, 68.6</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.9848484848484849</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9658246656760773</v>
+        <v>0.9390787518573551</v>
       </c>
       <c r="C7" t="n">
-        <v>0.425</v>
+        <v>0.3970588235294117</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6296296296296297</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7977271476528535</v>
+        <v>0.9695393759286776</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9528571428571428</v>
+        <v>0.9414285714285714</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5074626865671642</v>
+        <v>0.5684210526315789</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>('Divisible_by_4=True', 'Divisible_by_10=True')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_10=True')</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_4=True AND Divisible_by_10=True</t>
+          <t>NOT_Divisible_by_2=True AND Divisible_by_10=True OR Divisible_by_2=True AND Divisible_by_10=True</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>0.9907407407407407</v>
       </c>
       <c r="B8" t="n">
-        <v>0.888558692421991</v>
+        <v>0.9539375928677564</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2647058823529412</v>
+        <v>0.4038461538461539</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9442793462109955</v>
+        <v>0.865857685322767</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.9471428571428572</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4186046511627907</v>
+        <v>0.5316455696202531</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>('Divisible_by_10=True', 'Number∈(68.6, 135.2]')</t>
+          <t>('Divisible_by_8=True', 'Divisible_by_10=True')</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_10=True AND Number∈(68.6, 135.2 OR Divisible_by_10=True AND NOT_Number∈(68.6, 135.2 OR Divisible_by_10=True AND Number∈(68.6, 135.2</t>
+          <t>NOT_Divisible_by_8=True AND Divisible_by_10=True</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.998330550918197</v>
+        <v>0.9892141756548536</v>
       </c>
       <c r="B9" t="n">
-        <v>0.888558692421991</v>
+        <v>0.9539375928677564</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2574257425742574</v>
+        <v>0.392156862745098</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9629629629629629</v>
+        <v>0.7407407407407407</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9257608276924769</v>
+        <v>0.8473391668042485</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8914285714285715</v>
+        <v>0.9457142857142857</v>
       </c>
       <c r="G9" t="n">
-        <v>0.40625</v>
+        <v>0.5128205128205128</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>('Divisible_by_10=True', 'Number∈(713.6, 782.6]')</t>
+          <t>('Divisible_by_7=True', 'Divisible_by_10=True')</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_10=True AND Number∈(713.6, 782.6 OR Divisible_by_10=True AND NOT_Number∈(713.6, 782.6</t>
+          <t>NOT_Divisible_by_7=True AND Divisible_by_10=True</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.9966777408637874</v>
+        <v>0.9848484848484849</v>
       </c>
       <c r="B10" t="n">
-        <v>0.8915304606240714</v>
+        <v>0.9658246656760773</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2551020408163265</v>
+        <v>0.425</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9087281932749985</v>
+        <v>0.7977271476528535</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.9528571428571428</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4</v>
+        <v>0.5074626865671642</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>('Divisible_by_10=True', 'Number∈(531.8, 594.4]')</t>
+          <t>('Divisible_by_4=True', 'Divisible_by_10=True')</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_10=True AND Number∈(531.8, 594.4 OR Divisible_by_10=True AND NOT_Number∈(531.8, 594.4</t>
+          <t>NOT_Divisible_by_4=True AND Divisible_by_10=True</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.984399375975039</v>
+        <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>0.937592867756315</v>
+        <v>0.888558692421991</v>
       </c>
       <c r="C11" t="n">
-        <v>0.288135593220339</v>
+        <v>0.2647058823529412</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6296296296296297</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7836112486929724</v>
+        <v>0.9442793462109955</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9257142857142857</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3953488372093023</v>
+        <v>0.4186046511627907</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>('Divisible_by_4=True', 'Divisible_by_6=True')</t>
+          <t>('Divisible_by_10=True', 'Number∈(68.6, 135.2]')</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_4=True AND Divisible_by_6=True</t>
+          <t>NOT_Divisible_by_10=True AND Number∈(68.6, 135.2 OR Divisible_by_10=True AND NOT_Number∈(68.6, 135.2 OR Divisible_by_10=True AND Number∈(68.6, 135.2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>0.998330550918197</v>
       </c>
       <c r="B12" t="n">
-        <v>0.8766716196136701</v>
+        <v>0.888558692421991</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2454545454545455</v>
+        <v>0.2574257425742574</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9383358098068351</v>
+        <v>0.9257608276924769</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8814285714285715</v>
+        <v>0.8914285714285715</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3941605839416059</v>
+        <v>0.40625</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>('Divisible_by_10=True', 'Number∈(338.0, 397.8]')</t>
+          <t>('Divisible_by_10=True', 'Number∈(713.6, 782.6]')</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -902,121 +902,121 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_10=True AND Number∈(338.0, 397.8 OR Divisible_by_10=True AND NOT_Number∈(338.0, 397.8</t>
+          <t>NOT_Divisible_by_10=True AND Number∈(713.6, 782.6 OR Divisible_by_10=True AND NOT_Number∈(713.6, 782.6</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>0.9966777408637874</v>
       </c>
       <c r="B13" t="n">
-        <v>0.87518573551263</v>
+        <v>0.8915304606240714</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2432432432432433</v>
+        <v>0.2551020408163265</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="E13" t="n">
-        <v>0.937592867756315</v>
+        <v>0.9087281932749985</v>
       </c>
       <c r="F13" t="n">
-        <v>0.88</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="G13" t="n">
-        <v>0.391304347826087</v>
+        <v>0.4</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>('Divisible_by_6=True', 'Number∈(258.0, 338.0]')</t>
+          <t>('Divisible_by_10=True', 'Number∈(531.8, 594.4]')</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Divisible_by_6=True AND NOT_Number∈(258.0, 338.0</t>
+          <t>NOT_Divisible_by_10=True AND Number∈(531.8, 594.4 OR Divisible_by_10=True AND NOT_Number∈(531.8, 594.4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>0.984399375975039</v>
       </c>
       <c r="B14" t="n">
-        <v>0.87518573551263</v>
+        <v>0.937592867756315</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2432432432432433</v>
+        <v>0.288135593220339</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="E14" t="n">
-        <v>0.937592867756315</v>
+        <v>0.7836112486929724</v>
       </c>
       <c r="F14" t="n">
-        <v>0.88</v>
+        <v>0.9257142857142857</v>
       </c>
       <c r="G14" t="n">
-        <v>0.391304347826087</v>
+        <v>0.3953488372093023</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>('Divisible_by_10=True', 'Number∈(2.999, 68.6]')</t>
+          <t>('Divisible_by_4=True', 'Divisible_by_6=True')</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_10=True AND Number∈(2.999, 68.6 OR Divisible_by_10=True AND NOT_Number∈(2.999, 68.6</t>
+          <t>NOT_Divisible_by_4=True AND Divisible_by_6=True</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.9901477832512315</v>
+        <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>0.8959881129271917</v>
+        <v>0.8766716196136701</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2307692307692308</v>
+        <v>0.2454545454545455</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7777777777777778</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8368829453524846</v>
+        <v>0.9383358098068351</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8914285714285715</v>
+        <v>0.8814285714285715</v>
       </c>
       <c r="G15" t="n">
-        <v>0.3559322033898305</v>
+        <v>0.3941605839416059</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>('Divisible_by_6=True', 'Divisible_by_8=True')</t>
+          <t>('Divisible_by_10=True', 'Number∈(338.0, 397.8]')</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Divisible_by_6=True AND NOT_Divisible_by_8=True</t>
+          <t>NOT_Divisible_by_10=True AND Number∈(338.0, 397.8 OR Divisible_by_10=True AND NOT_Number∈(338.0, 397.8</t>
         </is>
       </c>
     </row>
@@ -1025,26 +1025,26 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>0.8439821693907875</v>
+        <v>0.87518573551263</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2045454545454546</v>
+        <v>0.2432432432432433</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9219910846953938</v>
+        <v>0.937592867756315</v>
       </c>
       <c r="F16" t="n">
-        <v>0.85</v>
+        <v>0.88</v>
       </c>
       <c r="G16" t="n">
-        <v>0.339622641509434</v>
+        <v>0.391304347826087</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>('Divisible_by_5=True', 'Number∈(2.999, 68.6]')</t>
+          <t>('Divisible_by_6=True', 'Number∈(258.0, 338.0]')</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Divisible_by_5=True AND NOT_Number∈(2.999, 68.6</t>
+          <t>Divisible_by_6=True AND NOT_Number∈(258.0, 338.0</t>
         </is>
       </c>
     </row>
@@ -1063,36 +1063,36 @@
         <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>0.8410104011887073</v>
+        <v>0.87518573551263</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2014925373134328</v>
+        <v>0.2432432432432433</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9205052005943537</v>
+        <v>0.937592867756315</v>
       </c>
       <c r="F17" t="n">
-        <v>0.8471428571428572</v>
+        <v>0.88</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3354037267080745</v>
+        <v>0.391304347826087</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>('Divisible_by_9=True', 'Divisible_by_10=True')</t>
+          <t>('Divisible_by_10=True', 'Number∈(2.999, 68.6]')</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_9=True AND Divisible_by_10=True OR Divisible_by_9=True AND NOT_Divisible_by_10=True OR Divisible_by_9=True AND Divisible_by_10=True</t>
+          <t>NOT_Divisible_by_10=True AND Number∈(2.999, 68.6 OR Divisible_by_10=True AND NOT_Number∈(2.999, 68.6</t>
         </is>
       </c>
     </row>
@@ -1101,36 +1101,36 @@
         <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>0.8335809806835067</v>
+        <v>0.8736998514115899</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1942446043165468</v>
+        <v>0.2410714285714286</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9167904903417534</v>
+        <v>0.936849925705795</v>
       </c>
       <c r="F18" t="n">
-        <v>0.84</v>
+        <v>0.8785714285714286</v>
       </c>
       <c r="G18" t="n">
-        <v>0.3253012048192771</v>
+        <v>0.3884892086330935</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>('Divisible_by_8=True', 'Divisible_by_10=True')</t>
+          <t>('Divisible_by_6=True', 'Number∈(2.999, 68.6]')</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_8=True AND Divisible_by_10=True OR Divisible_by_8=True AND NOT_Divisible_by_10=True OR Divisible_by_8=True AND Divisible_by_10=True</t>
+          <t>Divisible_by_6=True AND NOT_Number∈(2.999, 68.6</t>
         </is>
       </c>
     </row>
@@ -1139,74 +1139,74 @@
         <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>0.8216939078751857</v>
+        <v>0.8677563150074294</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1836734693877551</v>
+        <v>0.2327586206896552</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9108469539375929</v>
+        <v>0.9338781575037147</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8285714285714286</v>
+        <v>0.8728571428571429</v>
       </c>
       <c r="G19" t="n">
-        <v>0.3103448275862069</v>
+        <v>0.3776223776223776</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>('Divisible_by_5=True', 'Divisible_by_6=True')</t>
+          <t>('Divisible_by_10=True', 'Number∈(2.999, 68.6]')</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Divisible_by_5=True AND NOT_Divisible_by_6=True OR Divisible_by_5=True AND Divisible_by_6=True</t>
+          <t>NOT_Divisible_by_10=True AND Number∈(2.999, 68.6 OR Divisible_by_10=True AND NOT_Number∈(2.999, 68.6 OR Divisible_by_10=True AND Number∈(2.999, 68.6</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.99644128113879</v>
+        <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>0.8320950965824666</v>
+        <v>0.8662704309063893</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1811594202898551</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9259259259259259</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8790105112541964</v>
+        <v>0.9331352154531947</v>
       </c>
       <c r="F20" t="n">
-        <v>0.8357142857142857</v>
+        <v>0.8714285714285714</v>
       </c>
       <c r="G20" t="n">
-        <v>0.303030303030303</v>
+        <v>0.375</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>('Divisible_by_6=True', 'Number∈(397.8, 471.2]')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_6=True AND Number∈(397.8, 471.2 OR Divisible_by_6=True AND NOT_Number∈(397.8, 471.2</t>
+          <t>Divisible_by_2=True AND Divisible_by_3=True</t>
         </is>
       </c>
     </row>
@@ -1215,36 +1215,36 @@
         <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>0.8112927191679049</v>
+        <v>0.8662704309063893</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1753246753246753</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="D21" t="n">
         <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9056463595839525</v>
+        <v>0.9331352154531947</v>
       </c>
       <c r="F21" t="n">
-        <v>0.8185714285714286</v>
+        <v>0.8714285714285714</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2983425414364641</v>
+        <v>0.375</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>('Divisible_by_6=True', 'Number∈(258.0, 338.0]')</t>
+          <t>('Divisible_by_6=True', 'Divisible_by_7=True')</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_6=True AND Number∈(258.0, 338.0 OR Divisible_by_6=True AND NOT_Number∈(258.0, 338.0</t>
+          <t>Divisible_by_6=True AND NOT_Divisible_by_7=True OR Divisible_by_6=True AND Divisible_by_7=True</t>
         </is>
       </c>
     </row>
@@ -1253,102 +1253,102 @@
         <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>0.8023774145616642</v>
+        <v>0.8662704309063893</v>
       </c>
       <c r="C22" t="n">
-        <v>0.16875</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9011887072808321</v>
+        <v>0.9331352154531947</v>
       </c>
       <c r="F22" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.8714285714285714</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2887700534759359</v>
+        <v>0.375</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>('Divisible_by_6=True', 'Number∈(2.999, 68.6]')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_6=True')</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_6=True AND Number∈(2.999, 68.6 OR Divisible_by_6=True AND NOT_Number∈(2.999, 68.6</t>
+          <t>NOT_Divisible_by_2=True AND Divisible_by_6=True OR Divisible_by_2=True AND Divisible_by_6=True</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>0.9901477832512315</v>
       </c>
       <c r="B23" t="n">
-        <v>0.787518573551263</v>
+        <v>0.8959881129271917</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1588235294117647</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="E23" t="n">
-        <v>0.8937592867756314</v>
+        <v>0.8368829453524846</v>
       </c>
       <c r="F23" t="n">
-        <v>0.7957142857142857</v>
+        <v>0.8914285714285715</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2741116751269035</v>
+        <v>0.3559322033898305</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>('Divisible_by_5=True', 'Number∈(2.999, 68.6]')</t>
+          <t>('Divisible_by_6=True', 'Divisible_by_8=True')</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_5=True AND Number∈(2.999, 68.6 OR Divisible_by_5=True AND NOT_Number∈(2.999, 68.6</t>
+          <t>Divisible_by_6=True AND NOT_Divisible_by_8=True</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.9879518072289156</v>
+        <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>0.8528974739970282</v>
+        <v>0.8439821693907875</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1680672268907563</v>
+        <v>0.2045454545454546</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7407407407407407</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>0.7968191073688845</v>
+        <v>0.9219910846953938</v>
       </c>
       <c r="F24" t="n">
-        <v>0.8485714285714285</v>
+        <v>0.85</v>
       </c>
       <c r="G24" t="n">
-        <v>0.273972602739726</v>
+        <v>0.339622641509434</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>('Divisible_by_5=True', 'Divisible_by_7=True')</t>
+          <t>('Divisible_by_5=True', 'Number∈(2.999, 68.6]')</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Divisible_by_5=True AND NOT_Divisible_by_7=True</t>
+          <t>Divisible_by_5=True AND NOT_Number∈(2.999, 68.6</t>
         </is>
       </c>
     </row>
@@ -1367,26 +1367,26 @@
         <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>0.7399702823179792</v>
+        <v>0.8410104011887073</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1336633663366337</v>
+        <v>0.2014925373134328</v>
       </c>
       <c r="D25" t="n">
         <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>0.8699851411589896</v>
+        <v>0.9205052005943537</v>
       </c>
       <c r="F25" t="n">
-        <v>0.75</v>
+        <v>0.8471428571428572</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2358078602620087</v>
+        <v>0.3354037267080745</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>('Divisible_by_5=True', 'Divisible_by_9=True')</t>
+          <t>('Divisible_by_9=True', 'Divisible_by_10=True')</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1396,45 +1396,45 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_5=True AND Divisible_by_9=True OR Divisible_by_5=True AND NOT_Divisible_by_9=True OR Divisible_by_5=True AND Divisible_by_9=True</t>
+          <t>NOT_Divisible_by_9=True AND Divisible_by_10=True OR Divisible_by_9=True AND NOT_Divisible_by_10=True OR Divisible_by_9=True AND Divisible_by_10=True</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.9827882960413081</v>
+        <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>0.8484398216939079</v>
+        <v>0.8335809806835067</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.1942446043165468</v>
       </c>
       <c r="D26" t="n">
-        <v>0.6296296296296297</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>0.7390347256617689</v>
+        <v>0.9167904903417534</v>
       </c>
       <c r="F26" t="n">
         <v>0.84</v>
       </c>
       <c r="G26" t="n">
-        <v>0.2328767123287671</v>
+        <v>0.3253012048192771</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>('Divisible_by_4=True', 'Divisible_by_5=True')</t>
+          <t>('Divisible_by_8=True', 'Divisible_by_10=True')</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_4=True AND Divisible_by_5=True</t>
+          <t>NOT_Divisible_by_8=True AND Divisible_by_10=True OR Divisible_by_8=True AND NOT_Divisible_by_10=True OR Divisible_by_8=True AND Divisible_by_10=True</t>
         </is>
       </c>
     </row>
@@ -1443,36 +1443,36 @@
         <v>1</v>
       </c>
       <c r="B27" t="n">
-        <v>0.7221396731054978</v>
+        <v>0.8216939078751857</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1261682242990654</v>
+        <v>0.1836734693877551</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>0.8610698365527489</v>
+        <v>0.9108469539375929</v>
       </c>
       <c r="F27" t="n">
-        <v>0.7328571428571429</v>
+        <v>0.8285714285714286</v>
       </c>
       <c r="G27" t="n">
-        <v>0.2240663900414938</v>
+        <v>0.3103448275862069</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>('Divisible_by_3=True', 'Number∈(2.999, 68.6]')</t>
+          <t>('Divisible_by_5=True', 'Divisible_by_6=True')</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Divisible_by_3=True AND NOT_Number∈(2.999, 68.6</t>
+          <t>Divisible_by_5=True AND NOT_Divisible_by_6=True OR Divisible_by_5=True AND Divisible_by_6=True</t>
         </is>
       </c>
     </row>
@@ -1481,150 +1481,150 @@
         <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>0.7161961367013373</v>
+        <v>0.8216939078751857</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1238532110091743</v>
+        <v>0.1836734693877551</v>
       </c>
       <c r="D28" t="n">
         <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>0.8580980683506687</v>
+        <v>0.9108469539375929</v>
       </c>
       <c r="F28" t="n">
-        <v>0.7271428571428571</v>
+        <v>0.8285714285714286</v>
       </c>
       <c r="G28" t="n">
-        <v>0.2204081632653061</v>
+        <v>0.3103448275862069</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>('Divisible_by_4=True', 'Divisible_by_10=True')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_5=True')</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_4=True AND Divisible_by_10=True OR Divisible_by_4=True AND NOT_Divisible_by_10=True OR Divisible_by_4=True AND Divisible_by_10=True</t>
+          <t>NOT_Divisible_by_2=True AND Divisible_by_5=True OR Divisible_by_2=True AND Divisible_by_5=True</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.9834254143646409</v>
+        <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>0.7934621099554234</v>
+        <v>0.8216939078751857</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1146496815286624</v>
+        <v>0.1836734693877551</v>
       </c>
       <c r="D29" t="n">
-        <v>0.6666666666666666</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>0.730064388311045</v>
+        <v>0.9108469539375929</v>
       </c>
       <c r="F29" t="n">
-        <v>0.7885714285714286</v>
+        <v>0.8285714285714286</v>
       </c>
       <c r="G29" t="n">
-        <v>0.1956521739130435</v>
+        <v>0.3103448275862069</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>('Divisible_by_3=True', 'Divisible_by_9=True')</t>
+          <t>('Divisible_by_5=True', 'Divisible_by_10=True')</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Divisible_by_3=True AND NOT_Divisible_by_9=True</t>
+          <t>NOT_Divisible_by_5=True AND Divisible_by_10=True OR Divisible_by_5=True AND NOT_Divisible_by_10=True OR Divisible_by_5=True AND Divisible_by_10=True</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.9862745098039216</v>
+        <v>0.99644128113879</v>
       </c>
       <c r="B30" t="n">
-        <v>0.7473997028231798</v>
+        <v>0.8320950965824666</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1052631578947368</v>
+        <v>0.1811594202898551</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7407407407407407</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="E30" t="n">
-        <v>0.7440702217819603</v>
+        <v>0.8790105112541964</v>
       </c>
       <c r="F30" t="n">
-        <v>0.7471428571428571</v>
+        <v>0.8357142857142857</v>
       </c>
       <c r="G30" t="n">
-        <v>0.184331797235023</v>
+        <v>0.303030303030303</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>('Divisible_by_3=True', 'Divisible_by_7=True')</t>
+          <t>('Divisible_by_6=True', 'Number∈(397.8, 471.2]')</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Divisible_by_3=True AND NOT_Divisible_by_7=True</t>
+          <t>NOT_Divisible_by_6=True AND Number∈(397.8, 471.2 OR Divisible_by_6=True AND NOT_Number∈(397.8, 471.2</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.9814814814814815</v>
+        <v>1</v>
       </c>
       <c r="B31" t="n">
-        <v>0.787518573551263</v>
+        <v>0.8112927191679049</v>
       </c>
       <c r="C31" t="n">
-        <v>0.10625</v>
+        <v>0.1753246753246753</v>
       </c>
       <c r="D31" t="n">
-        <v>0.6296296296296297</v>
+        <v>1</v>
       </c>
       <c r="E31" t="n">
-        <v>0.7085741015904464</v>
+        <v>0.9056463595839525</v>
       </c>
       <c r="F31" t="n">
-        <v>0.7814285714285715</v>
+        <v>0.8185714285714286</v>
       </c>
       <c r="G31" t="n">
-        <v>0.1818181818181818</v>
+        <v>0.2983425414364641</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Divisible_by_4=True')</t>
+          <t>('Divisible_by_6=True', 'Number∈(258.0, 338.0]')</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Divisible_by_2=True AND NOT_Divisible_by_4=True</t>
+          <t>NOT_Divisible_by_6=True AND Number∈(258.0, 338.0 OR Divisible_by_6=True AND NOT_Number∈(258.0, 338.0</t>
         </is>
       </c>
     </row>
@@ -1633,36 +1633,36 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>0.5542347696879644</v>
+        <v>0.8023774145616642</v>
       </c>
       <c r="C32" t="n">
-        <v>0.08256880733944955</v>
+        <v>0.16875</v>
       </c>
       <c r="D32" t="n">
         <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>0.7771173848439822</v>
+        <v>0.9011887072808321</v>
       </c>
       <c r="F32" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="G32" t="n">
-        <v>0.1525423728813559</v>
+        <v>0.2887700534759359</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>('Divisible_by_3=True', 'Divisible_by_5=True')</t>
+          <t>('Divisible_by_6=True', 'Number∈(2.999, 68.6]')</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_3=True AND Divisible_by_5=True OR Divisible_by_3=True AND NOT_Divisible_by_5=True OR Divisible_by_3=True AND Divisible_by_5=True</t>
+          <t>NOT_Divisible_by_6=True AND Number∈(2.999, 68.6 OR Divisible_by_6=True AND NOT_Number∈(2.999, 68.6</t>
         </is>
       </c>
     </row>
@@ -1671,74 +1671,74 @@
         <v>1</v>
       </c>
       <c r="B33" t="n">
-        <v>0.537890044576523</v>
+        <v>0.787518573551263</v>
       </c>
       <c r="C33" t="n">
-        <v>0.07988165680473373</v>
+        <v>0.1588235294117647</v>
       </c>
       <c r="D33" t="n">
         <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>0.7689450222882614</v>
+        <v>0.8937592867756314</v>
       </c>
       <c r="F33" t="n">
-        <v>0.5557142857142857</v>
+        <v>0.7957142857142857</v>
       </c>
       <c r="G33" t="n">
-        <v>0.1479452054794521</v>
+        <v>0.2741116751269035</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+          <t>('Divisible_by_5=True', 'Number∈(2.999, 68.6]')</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
+          <t>NOT_Divisible_by_5=True AND Number∈(2.999, 68.6 OR Divisible_by_5=True AND NOT_Number∈(2.999, 68.6</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1</v>
+        <v>0.9879518072289156</v>
       </c>
       <c r="B34" t="n">
-        <v>0.5185735512630015</v>
+        <v>0.8528974739970282</v>
       </c>
       <c r="C34" t="n">
-        <v>0.07692307692307693</v>
+        <v>0.1680672268907563</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>0.7407407407407407</v>
       </c>
       <c r="E34" t="n">
-        <v>0.7592867756315007</v>
+        <v>0.7968191073688845</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5371428571428571</v>
+        <v>0.8485714285714285</v>
       </c>
       <c r="G34" t="n">
-        <v>0.1428571428571429</v>
+        <v>0.273972602739726</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Divisible_by_5=True')</t>
+          <t>('Divisible_by_5=True', 'Divisible_by_7=True')</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_5=True OR Divisible_by_2=True AND Divisible_by_5=True</t>
+          <t>Divisible_by_5=True AND NOT_Divisible_by_7=True</t>
         </is>
       </c>
     </row>
@@ -1747,74 +1747,74 @@
         <v>1</v>
       </c>
       <c r="B35" t="n">
-        <v>0.4992570579494799</v>
+        <v>0.7399702823179792</v>
       </c>
       <c r="C35" t="n">
-        <v>0.07417582417582418</v>
+        <v>0.1336633663366337</v>
       </c>
       <c r="D35" t="n">
         <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>0.74962852897474</v>
+        <v>0.8699851411589896</v>
       </c>
       <c r="F35" t="n">
-        <v>0.5185714285714286</v>
+        <v>0.75</v>
       </c>
       <c r="G35" t="n">
-        <v>0.1381074168797954</v>
+        <v>0.2358078602620087</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+          <t>('Divisible_by_5=True', 'Divisible_by_9=True')</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
+          <t>NOT_Divisible_by_5=True AND Divisible_by_9=True OR Divisible_by_5=True AND NOT_Divisible_by_9=True OR Divisible_by_5=True AND Divisible_by_9=True</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1</v>
+        <v>0.9827882960413081</v>
       </c>
       <c r="B36" t="n">
-        <v>0.4011887072808321</v>
+        <v>0.8484398216939079</v>
       </c>
       <c r="C36" t="n">
-        <v>0.06279069767441861</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="E36" t="n">
-        <v>0.700594353640416</v>
+        <v>0.7390347256617689</v>
       </c>
       <c r="F36" t="n">
-        <v>0.4242857142857143</v>
+        <v>0.84</v>
       </c>
       <c r="G36" t="n">
-        <v>0.1181619256017506</v>
+        <v>0.2328767123287671</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Divisible_by_5=True')</t>
+          <t>('Divisible_by_4=True', 'Divisible_by_5=True')</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_5=True OR NOT_Divisible_by_2=True AND Divisible_by_5=True OR Divisible_by_2=True AND Divisible_by_5=True</t>
+          <t>NOT_Divisible_by_4=True AND Divisible_by_5=True</t>
         </is>
       </c>
     </row>
@@ -1823,36 +1823,36 @@
         <v>1</v>
       </c>
       <c r="B37" t="n">
-        <v>0.3670133729569093</v>
+        <v>0.7221396731054978</v>
       </c>
       <c r="C37" t="n">
-        <v>0.05960264900662252</v>
+        <v>0.1261682242990654</v>
       </c>
       <c r="D37" t="n">
         <v>1</v>
       </c>
       <c r="E37" t="n">
-        <v>0.6835066864784547</v>
+        <v>0.8610698365527489</v>
       </c>
       <c r="F37" t="n">
-        <v>0.3914285714285714</v>
+        <v>0.7328571428571429</v>
       </c>
       <c r="G37" t="n">
-        <v>0.1125</v>
+        <v>0.2240663900414938</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+          <t>('Divisible_by_3=True', 'Number∈(2.999, 68.6]')</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND Divisible_by_3=True OR Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
+          <t>Divisible_by_3=True AND NOT_Number∈(2.999, 68.6</t>
         </is>
       </c>
     </row>
@@ -1861,36 +1861,36 @@
         <v>1</v>
       </c>
       <c r="B38" t="n">
-        <v>0.3283803863298663</v>
+        <v>0.7161961367013373</v>
       </c>
       <c r="C38" t="n">
-        <v>0.05636743215031315</v>
+        <v>0.1238532110091743</v>
       </c>
       <c r="D38" t="n">
         <v>1</v>
       </c>
       <c r="E38" t="n">
-        <v>0.6641901931649332</v>
+        <v>0.8580980683506687</v>
       </c>
       <c r="F38" t="n">
-        <v>0.3542857142857143</v>
+        <v>0.7271428571428571</v>
       </c>
       <c r="G38" t="n">
-        <v>0.1067193675889328</v>
+        <v>0.2204081632653061</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+          <t>('Divisible_by_4=True', 'Divisible_by_10=True')</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR NOT_Divisible_by_2=True AND Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
+          <t>NOT_Divisible_by_4=True AND Divisible_by_10=True OR Divisible_by_4=True AND NOT_Divisible_by_10=True OR Divisible_by_4=True AND Divisible_by_10=True</t>
         </is>
       </c>
     </row>
@@ -1899,22 +1899,22 @@
         <v>1</v>
       </c>
       <c r="B39" t="n">
-        <v>0.1783060921248143</v>
+        <v>0.6953937592867756</v>
       </c>
       <c r="C39" t="n">
-        <v>0.04655172413793104</v>
+        <v>0.1163793103448276</v>
       </c>
       <c r="D39" t="n">
         <v>1</v>
       </c>
       <c r="E39" t="n">
-        <v>0.5891530460624071</v>
+        <v>0.8476968796433878</v>
       </c>
       <c r="F39" t="n">
-        <v>0.21</v>
+        <v>0.7071428571428572</v>
       </c>
       <c r="G39" t="n">
-        <v>0.08896210873146623</v>
+        <v>0.2084942084942085</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -1923,12 +1923,12 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_3=True AND NOT_Divisible_by_4=True OR Divisible_by_3=True AND NOT_Divisible_by_4=True OR Divisible_by_3=True AND Divisible_by_4=True</t>
+          <t>Divisible_by_3=True AND NOT_Divisible_by_4=True OR Divisible_by_3=True AND Divisible_by_4=True</t>
         </is>
       </c>
     </row>
@@ -1937,22 +1937,22 @@
         <v>1</v>
       </c>
       <c r="B40" t="n">
-        <v>0.1708766716196137</v>
+        <v>0.6953937592867756</v>
       </c>
       <c r="C40" t="n">
-        <v>0.04615384615384616</v>
+        <v>0.1163793103448276</v>
       </c>
       <c r="D40" t="n">
         <v>1</v>
       </c>
       <c r="E40" t="n">
-        <v>0.5854383358098068</v>
+        <v>0.8476968796433878</v>
       </c>
       <c r="F40" t="n">
-        <v>0.2028571428571428</v>
+        <v>0.7071428571428572</v>
       </c>
       <c r="G40" t="n">
-        <v>0.08823529411764706</v>
+        <v>0.2084942084942085</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -1961,12 +1961,12 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
+          <t>NOT_Divisible_by_2=True AND Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
         </is>
       </c>
     </row>
@@ -1975,402 +1975,402 @@
         <v>1</v>
       </c>
       <c r="B41" t="n">
-        <v>0.1515601783060921</v>
+        <v>0.6953937592867756</v>
       </c>
       <c r="C41" t="n">
-        <v>0.0451505016722408</v>
+        <v>0.1163793103448276</v>
       </c>
       <c r="D41" t="n">
         <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>0.575780089153046</v>
+        <v>0.8476968796433878</v>
       </c>
       <c r="F41" t="n">
-        <v>0.1842857142857143</v>
+        <v>0.7071428571428572</v>
       </c>
       <c r="G41" t="n">
-        <v>0.08639999999999999</v>
+        <v>0.2084942084942085</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>('Number∈(2.999, 68.6]', 'Number∈(258.0, 338.0]')</t>
+          <t>('Divisible_by_3=True', 'Divisible_by_6=True')</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>NOT_Number∈(2.999, 68.6 AND NOT_Number∈(258.0, 338.0</t>
+          <t>NOT_Divisible_by_3=True AND Divisible_by_6=True OR Divisible_by_3=True AND NOT_Divisible_by_6=True OR Divisible_by_3=True AND Divisible_by_6=True</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.9809523809523809</v>
+        <v>0.9834254143646409</v>
       </c>
       <c r="B42" t="n">
-        <v>0.1530460624071323</v>
+        <v>0.7934621099554234</v>
       </c>
       <c r="C42" t="n">
-        <v>0.04201680672268908</v>
+        <v>0.1146496815286624</v>
       </c>
       <c r="D42" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5394859941665291</v>
+        <v>0.730064388311045</v>
       </c>
       <c r="F42" t="n">
-        <v>0.1828571428571429</v>
+        <v>0.7885714285714286</v>
       </c>
       <c r="G42" t="n">
-        <v>0.08038585209003217</v>
+        <v>0.1956521739130435</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>('Number∈(2.999, 68.6]', 'Number∈(135.2, 201.0]')</t>
+          <t>('Divisible_by_3=True', 'Divisible_by_9=True')</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>NOT_Number∈(2.999, 68.6 AND NOT_Number∈(135.2, 201.0</t>
+          <t>Divisible_by_3=True AND NOT_Divisible_by_9=True</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1</v>
+        <v>0.9834254143646409</v>
       </c>
       <c r="B43" t="n">
-        <v>0.03714710252600297</v>
+        <v>0.7934621099554234</v>
       </c>
       <c r="C43" t="n">
-        <v>0.04</v>
+        <v>0.1146496815286624</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E43" t="n">
-        <v>0.5185735512630014</v>
+        <v>0.730064388311045</v>
       </c>
       <c r="F43" t="n">
-        <v>0.07428571428571429</v>
+        <v>0.7885714285714286</v>
       </c>
       <c r="G43" t="n">
-        <v>0.07692307692307693</v>
+        <v>0.1956521739130435</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Number∈(2.999, 68.6]')</t>
+          <t>('Divisible_by_3=True', 'Divisible_by_9=True')</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND NOT_Number∈(2.999, 68.6 OR NOT_Divisible_by_2=True AND Number∈(2.999, 68.6 OR Divisible_by_2=True AND NOT_Number∈(2.999, 68.6</t>
+          <t>NOT_Divisible_by_3=True AND Divisible_by_9=True OR Divisible_by_3=True AND NOT_Divisible_by_9=True</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.956989247311828</v>
+        <v>0.9862745098039216</v>
       </c>
       <c r="B44" t="n">
-        <v>0.1322436849925706</v>
+        <v>0.7473997028231798</v>
       </c>
       <c r="C44" t="n">
-        <v>0.03789126853377265</v>
+        <v>0.1052631578947368</v>
       </c>
       <c r="D44" t="n">
-        <v>0.8518518518518519</v>
+        <v>0.7407407407407407</v>
       </c>
       <c r="E44" t="n">
-        <v>0.4920477684222112</v>
+        <v>0.7440702217819603</v>
       </c>
       <c r="F44" t="n">
-        <v>0.16</v>
+        <v>0.7471428571428571</v>
       </c>
       <c r="G44" t="n">
-        <v>0.0725552050473186</v>
+        <v>0.184331797235023</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>('Number∈(2.999, 68.6]', 'Number∈(68.6, 135.2]')</t>
+          <t>('Divisible_by_3=True', 'Divisible_by_7=True')</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>NOT_Number∈(2.999, 68.6 AND NOT_Number∈(68.6, 135.2</t>
+          <t>Divisible_by_3=True AND NOT_Divisible_by_7=True</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.9545454545454546</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="B45" t="n">
-        <v>0.187221396731055</v>
+        <v>0.787518573551263</v>
       </c>
       <c r="C45" t="n">
-        <v>0.03697183098591549</v>
+        <v>0.10625</v>
       </c>
       <c r="D45" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="E45" t="n">
-        <v>0.4824995872544163</v>
+        <v>0.7085741015904464</v>
       </c>
       <c r="F45" t="n">
-        <v>0.21</v>
+        <v>0.7814285714285715</v>
       </c>
       <c r="G45" t="n">
-        <v>0.07058823529411765</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>('Divisible_by_8=True', 'Number∈(2.999, 68.6]')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_4=True')</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_8=True AND NOT_Number∈(2.999, 68.6</t>
+          <t>Divisible_by_2=True AND NOT_Divisible_by_4=True</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.9559748427672956</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="B46" t="n">
-        <v>0.2258543833580981</v>
+        <v>0.787518573551263</v>
       </c>
       <c r="C46" t="n">
-        <v>0.03696857670979668</v>
+        <v>0.10625</v>
       </c>
       <c r="D46" t="n">
-        <v>0.7407407407407407</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="E46" t="n">
-        <v>0.4832975620494194</v>
+        <v>0.7085741015904464</v>
       </c>
       <c r="F46" t="n">
-        <v>0.2457142857142857</v>
+        <v>0.7814285714285715</v>
       </c>
       <c r="G46" t="n">
-        <v>0.07042253521126761</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>('Divisible_by_7=True', 'Number∈(2.999, 68.6]')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_4=True')</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_7=True AND NOT_Number∈(2.999, 68.6</t>
+          <t>NOT_Divisible_by_2=True AND Divisible_by_4=True OR Divisible_by_2=True AND NOT_Divisible_by_4=True</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.9541284403669725</v>
+        <v>1</v>
       </c>
       <c r="B47" t="n">
-        <v>0.3090638930163447</v>
+        <v>0.5542347696879644</v>
       </c>
       <c r="C47" t="n">
-        <v>0.03526970954356846</v>
+        <v>0.08256880733944955</v>
       </c>
       <c r="D47" t="n">
-        <v>0.6296296296296297</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>0.4693467613229872</v>
+        <v>0.7771173848439822</v>
       </c>
       <c r="F47" t="n">
-        <v>0.3214285714285715</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G47" t="n">
-        <v>0.06679764243614932</v>
+        <v>0.1525423728813559</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>('Divisible_by_4=True', 'Number∈(2.999, 68.6]')</t>
+          <t>('Divisible_by_3=True', 'Divisible_by_5=True')</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_4=True AND NOT_Number∈(2.999, 68.6</t>
+          <t>NOT_Divisible_by_3=True AND Divisible_by_5=True OR Divisible_by_3=True AND NOT_Divisible_by_5=True OR Divisible_by_3=True AND Divisible_by_5=True</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.9420849420849421</v>
+        <v>1</v>
       </c>
       <c r="B48" t="n">
-        <v>0.362555720653789</v>
+        <v>0.537890044576523</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0272108843537415</v>
+        <v>0.07988165680473373</v>
       </c>
       <c r="D48" t="n">
-        <v>0.4444444444444444</v>
+        <v>1</v>
       </c>
       <c r="E48" t="n">
-        <v>0.4035000825491167</v>
+        <v>0.7689450222882614</v>
       </c>
       <c r="F48" t="n">
-        <v>0.3657142857142857</v>
+        <v>0.5557142857142857</v>
       </c>
       <c r="G48" t="n">
-        <v>0.05128205128205128</v>
+        <v>0.1479452054794521</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>('Divisible_by_4=True', 'Divisible_by_7=True')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_4=True AND NOT_Divisible_by_7=True</t>
+          <t>Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.9436325678496869</v>
+        <v>1</v>
       </c>
       <c r="B49" t="n">
-        <v>0.6716196136701337</v>
+        <v>0.537890044576523</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>0.07988165680473373</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>0.3358098068350669</v>
+        <v>0.7689450222882614</v>
       </c>
       <c r="F49" t="n">
-        <v>0.6457142857142857</v>
+        <v>0.5557142857142857</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>0.1479452054794521</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_4=True')</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Divisible_by_2=True AND NOT_Divisible_by_3=True</t>
+          <t>NOT_Divisible_by_2=True AND Divisible_by_4=True OR Divisible_by_2=True AND NOT_Divisible_by_4=True OR Divisible_by_2=True AND Divisible_by_4=True</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.9538461538461539</v>
+        <v>1</v>
       </c>
       <c r="B50" t="n">
-        <v>0.8291233283803864</v>
+        <v>0.5185735512630015</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
-        <v>0.4145616641901931</v>
+        <v>0.7592867756315007</v>
       </c>
       <c r="F50" t="n">
-        <v>0.7971428571428572</v>
+        <v>0.5371428571428571</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>0.1428571428571429</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_5=True')</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND Divisible_by_3=True</t>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_5=True OR Divisible_by_2=True AND Divisible_by_5=True</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.9258241758241759</v>
+        <v>1</v>
       </c>
       <c r="B51" t="n">
-        <v>0.5007429420505201</v>
+        <v>0.4992570579494799</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>0.07417582417582418</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51" t="n">
-        <v>0.25037147102526</v>
+        <v>0.74962852897474</v>
       </c>
       <c r="F51" t="n">
-        <v>0.4814285714285714</v>
+        <v>0.5185714285714286</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>0.1381074168797954</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -2379,74 +2379,74 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND Divisible_by_3=True OR Divisible_by_2=True AND NOT_Divisible_by_3=True</t>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0.9403973509933775</v>
+        <v>1</v>
       </c>
       <c r="B52" t="n">
-        <v>0.6329866270430906</v>
+        <v>0.4011887072808321</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>0.06279069767441861</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" t="n">
-        <v>0.3164933135215453</v>
+        <v>0.700594353640416</v>
       </c>
       <c r="F52" t="n">
-        <v>0.6085714285714285</v>
+        <v>0.4242857142857143</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>0.1181619256017506</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+          <t>('Divisible_by_2=True', 'Divisible_by_5=True')</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True</t>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_5=True OR NOT_Divisible_by_2=True AND Divisible_by_5=True OR Divisible_by_2=True AND Divisible_by_5=True</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0.8836206896551724</v>
+        <v>1</v>
       </c>
       <c r="B53" t="n">
-        <v>0.3046062407132243</v>
+        <v>0.3670133729569093</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>0.05960264900662252</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>0.1523031203566122</v>
+        <v>0.6835066864784547</v>
       </c>
       <c r="F53" t="n">
-        <v>0.2928571428571429</v>
+        <v>0.3914285714285714</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>0.1125</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -2455,36 +2455,36 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND NOT_Divisible_by_3=True</t>
+          <t>NOT_Divisible_by_2=True AND Divisible_by_3=True OR Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.9201183431952663</v>
+        <v>1</v>
       </c>
       <c r="B54" t="n">
-        <v>0.462109955423477</v>
+        <v>0.3283803863298663</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>0.05636743215031315</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>0.2310549777117385</v>
+        <v>0.6641901931649332</v>
       </c>
       <c r="F54" t="n">
-        <v>0.4442857142857143</v>
+        <v>0.3542857142857143</v>
       </c>
       <c r="G54" t="n">
-        <v>0</v>
+        <v>0.1067193675889328</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -2493,48 +2493,1112 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]]</t>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR NOT_Divisible_by_2=True AND Divisible_by_3=True</t>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR NOT_Divisible_by_2=True AND Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
+        <v>1</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.1783060921248143</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.04655172413793104</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.5891530460624071</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.08896210873146623</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>('Divisible_by_3=True', 'Divisible_by_4=True')</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_3=True AND NOT_Divisible_by_4=True OR Divisible_by_3=True AND NOT_Divisible_by_4=True OR Divisible_by_3=True AND Divisible_by_4=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>1</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.1708766716196137</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.5854383358098068</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.2028571428571428</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.08823529411764706</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>1</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.1515601783060921</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.0451505016722408</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.575780089153046</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.1842857142857143</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.08639999999999999</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>('Number∈(2.999, 68.6]', 'Number∈(258.0, 338.0]')</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>NOT_Number∈(2.999, 68.6 AND NOT_Number∈(258.0, 338.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>0.9809523809523809</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.1530460624071323</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.04201680672268908</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.9259259259259259</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.5394859941665291</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.1828571428571429</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.08038585209003217</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>('Number∈(2.999, 68.6]', 'Number∈(135.2, 201.0]')</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>NOT_Number∈(2.999, 68.6 AND NOT_Number∈(135.2, 201.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>1</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.0787518573551263</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.04173106646058733</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.5393759286775632</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.1142857142857143</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.08011869436201782</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Number∈(2.999, 68.6]')</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Number∈(2.999, 68.6 OR Divisible_by_2=True AND NOT_Number∈(2.999, 68.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>1</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.0787518573551263</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.04173106646058733</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.5393759286775632</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.1142857142857143</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.08011869436201782</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>('Number∈(2.999, 68.6]', 'Number∈(68.6, 135.2]')</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>NOT_Number∈(2.999, 68.6 AND NOT_Number∈(68.6, 135.2 OR NOT_Number∈(2.999, 68.6 AND Number∈(68.6, 135.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.03714710252600297</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.5185735512630014</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.07428571428571429</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.07692307692307693</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Number∈(2.999, 68.6]')</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Number∈(2.999, 68.6 OR NOT_Divisible_by_2=True AND Number∈(2.999, 68.6 OR Divisible_by_2=True AND NOT_Number∈(2.999, 68.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>0</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.03857142857142857</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.03857142857142857</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.07427785419532325</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR NOT_Divisible_by_2=True AND Divisible_by_3=True OR Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND Divisible_by_3=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>0.956989247311828</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.1322436849925706</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.03789126853377265</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.8518518518518519</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.4920477684222112</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.0725552050473186</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>('Number∈(2.999, 68.6]', 'Number∈(68.6, 135.2]')</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>NOT_Number∈(2.999, 68.6 AND NOT_Number∈(68.6, 135.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>0.9545454545454546</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.187221396731055</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.03697183098591549</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.4824995872544163</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.07058823529411765</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>('Divisible_by_8=True', 'Number∈(2.999, 68.6]')</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_8=True AND NOT_Number∈(2.999, 68.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>0.9559748427672956</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.2258543833580981</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.03696857670979668</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.4832975620494194</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.2457142857142857</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.07042253521126761</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>('Divisible_by_7=True', 'Number∈(2.999, 68.6]')</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_7=True AND NOT_Number∈(2.999, 68.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>0.9541284403669725</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.3090638930163447</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.03526970954356846</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.6296296296296297</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.4693467613229872</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.3214285714285715</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.06679764243614932</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>('Divisible_by_4=True', 'Number∈(2.999, 68.6]')</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_4=True AND NOT_Number∈(2.999, 68.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>0.9310344827586207</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.1203566121842496</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.03425774877650897</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.4490671949810137</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.1457142857142857</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.065625</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_8=True')</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_8=True OR Divisible_by_2=True AND NOT_Divisible_by_8=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>0.9310344827586207</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.1203566121842496</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.03425774877650897</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.4490671949810137</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.1457142857142857</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.065625</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>('Divisible_by_8=True', 'Divisible_by_9=True')</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_8=True AND NOT_Divisible_by_9=True OR NOT_Divisible_by_8=True AND Divisible_by_9=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>0.9310344827586207</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.1203566121842496</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.03425774877650897</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.4490671949810137</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.1457142857142857</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.065625</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_8=True')</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_8=True OR NOT_Divisible_by_2=True AND Divisible_by_8=True OR Divisible_by_2=True AND NOT_Divisible_by_8=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>0.9385964912280702</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.1589895988112927</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.03412969283276451</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.4498651697760167</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.1814285714285714</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.06525285481239805</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_7=True')</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_7=True OR Divisible_by_2=True AND NOT_Divisible_by_7=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>0.9385964912280702</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.1589895988112927</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.03412969283276451</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.4498651697760167</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.1814285714285714</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.06525285481239805</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>('Divisible_by_7=True', 'Divisible_by_8=True')</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_7=True AND NOT_Divisible_by_8=True OR NOT_Divisible_by_7=True AND Divisible_by_8=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>0.9438202247191011</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.24962852897474</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.03256704980842912</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.6296296296296297</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.4396290793021849</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.2642857142857143</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.06193078324225865</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>('Divisible_by_4=True', 'Divisible_by_8=True')</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_4=True AND NOT_Divisible_by_8=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>0.9438202247191011</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.24962852897474</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.03256704980842912</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.6296296296296297</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.4396290793021849</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.2642857142857143</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.06193078324225865</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_4=True')</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_4=True OR Divisible_by_2=True AND NOT_Divisible_by_4=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>0.9438202247191011</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.24962852897474</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.03256704980842912</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.6296296296296297</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.4396290793021849</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.2642857142857143</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.06193078324225865</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>('Divisible_by_4=True', 'Divisible_by_5=True')</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_4=True AND NOT_Divisible_by_5=True OR NOT_Divisible_by_4=True AND Divisible_by_5=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>0.9438202247191011</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.24962852897474</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.03256704980842912</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.6296296296296297</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.4396290793021849</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.2642857142857143</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.06193078324225865</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_4=True')</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_4=True OR NOT_Divisible_by_2=True AND Divisible_by_4=True OR Divisible_by_2=True AND NOT_Divisible_by_4=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>0.9420849420849421</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.362555720653789</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.0272108843537415</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.4035000825491167</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.3657142857142857</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>('Divisible_by_4=True', 'Divisible_by_7=True')</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_4=True AND NOT_Divisible_by_7=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>0.9436325678496869</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.6716196136701337</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.3358098068350669</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.6457142857142857</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Divisible_by_2=True AND NOT_Divisible_by_3=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>0.9538461538461539</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.8291233283803864</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.4145616641901931</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.7971428571428572</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND Divisible_by_3=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>0.9258241758241759</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.5007429420505201</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.25037147102526</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.4814285714285714</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND Divisible_by_3=True OR Divisible_by_2=True AND NOT_Divisible_by_3=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>0.9403973509933775</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.6329866270430906</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.3164933135215453</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.6085714285714285</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>0.8836206896551724</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.3046062407132243</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.1523031203566122</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.2928571428571429</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR Divisible_by_2=True AND NOT_Divisible_by_3=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>0.9201183431952663</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.462109955423477</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.2310549777117385</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.4442857142857143</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]]</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR NOT_Divisible_by_2=True AND Divisible_by_3=True</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
         <v>0.7692307692307693</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B83" t="n">
         <v>0.1337295690936107</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C83" t="n">
         <v>0</v>
       </c>
-      <c r="D55" t="n">
+      <c r="D83" t="n">
         <v>0</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E83" t="n">
         <v>0.06686478454680533</v>
       </c>
-      <c r="F55" t="n">
+      <c r="F83" t="n">
         <v>0.1285714285714286</v>
       </c>
-      <c r="G55" t="n">
+      <c r="G83" t="n">
         <v>0</v>
       </c>
-      <c r="H55" t="inlineStr">
+      <c r="H83" t="inlineStr">
         <is>
           <t>('Divisible_by_2=True', 'Divisible_by_3=True')</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr">
+      <c r="I83" t="inlineStr">
         <is>
           <t>~df[columns[0]] &amp; ~df[columns[1]] | ~df[columns[0]] &amp; df[columns[1]] | df[columns[0]] &amp; ~df[columns[1]]</t>
         </is>
       </c>
-      <c r="J55" t="inlineStr">
+      <c r="J83" t="inlineStr">
         <is>
           <t>NOT_Divisible_by_2=True AND NOT_Divisible_by_3=True OR NOT_Divisible_by_2=True AND Divisible_by_3=True OR Divisible_by_2=True AND NOT_Divisible_by_3=True</t>
         </is>

</xml_diff>